<commit_message>
Casi la Primera Face completa
</commit_message>
<xml_diff>
--- a/Documentacion/Configuración de Plantillas SISIA.xlsx
+++ b/Documentacion/Configuración de Plantillas SISIA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\margarita.garcia.c\Documents\TESTING SENASICA\NUEVO DESARROLLO\siuce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SISIA\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7176" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7176" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos IE" sheetId="5" r:id="rId1"/>
@@ -1076,7 +1076,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1555,7 +1555,7 @@
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="56.33203125" customWidth="1"/>
     <col min="3" max="3" width="51.5546875" customWidth="1"/>
@@ -1569,7 +1569,7 @@
     <col min="12" max="12" width="28.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="40.200000000000003" customHeight="1">
       <c r="B2" s="29" t="s">
         <v>278</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="88.8" customHeight="1">
       <c r="B3" s="26" t="s">
         <v>339</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="118.8">
       <c r="B4" s="26" t="s">
         <v>337</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12">
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="28">
@@ -1701,7 +1701,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="28">
@@ -1730,7 +1730,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="28">
@@ -1759,7 +1759,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="28">
@@ -1788,7 +1788,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="28">
@@ -1817,7 +1817,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="28">
@@ -1846,7 +1846,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="28">
@@ -1875,7 +1875,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="28">
@@ -1904,7 +1904,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="28">
@@ -1943,11 +1943,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
@@ -1961,10 +1961,10 @@
     <col min="11" max="11" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2521,94 +2521,94 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11">
       <c r="H18" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11">
       <c r="G21" t="str">
         <f>CONCATENATE(B21,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11">
       <c r="G22" t="str">
         <f>CONCATENATE(B22,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11">
       <c r="G23" t="str">
         <f>CONCATENATE(B23,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11">
       <c r="G24" t="str">
         <f>CONCATENATE(B24,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11">
       <c r="G25" t="str">
         <f>CONCATENATE(B25,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11">
       <c r="G26" t="str">
         <f>CONCATENATE(B26,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11">
       <c r="G27" t="str">
         <f>CONCATENATE(B27,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11">
       <c r="G28" t="str">
         <f>CONCATENATE(B28,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11">
       <c r="G29" t="str">
         <f>CONCATENATE(B29,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11">
       <c r="G30" t="str">
         <f>CONCATENATE(B30,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11">
       <c r="G31" t="str">
         <f>CONCATENATE(B31,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11">
       <c r="G32" t="str">
         <f>CONCATENATE(B32,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:7">
       <c r="G33" t="str">
         <f>CONCATENATE(B33,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:7">
       <c r="G34" t="str">
         <f>CONCATENATE(B34,F19)</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:7">
       <c r="G35" t="str">
         <f>CONCATENATE(B35,F19)</f>
         <v/>
@@ -2631,7 +2631,7 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="30.109375" customWidth="1"/>
     <col min="4" max="4" width="34.77734375" customWidth="1"/>
@@ -2641,7 +2641,7 @@
     <col min="8" max="8" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11">
       <c r="C2" s="10" t="s">
         <v>132</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11">
       <c r="B3">
         <v>1</v>
       </c>
@@ -2697,7 +2697,7 @@
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11">
       <c r="B4">
         <v>2</v>
       </c>
@@ -2724,7 +2724,7 @@
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11">
       <c r="B5">
         <v>3</v>
       </c>
@@ -2751,7 +2751,7 @@
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
-    <row r="6" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="28.8">
       <c r="B6">
         <v>4</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11">
       <c r="B7">
         <v>5</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11">
       <c r="B8">
         <v>6</v>
       </c>
@@ -2832,7 +2832,7 @@
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11">
       <c r="B9">
         <v>7</v>
       </c>
@@ -2859,7 +2859,7 @@
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="28.8">
       <c r="B10">
         <v>8</v>
       </c>
@@ -2886,7 +2886,7 @@
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11">
       <c r="B11">
         <v>9</v>
       </c>
@@ -2913,7 +2913,7 @@
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11">
       <c r="B12">
         <v>10</v>
       </c>
@@ -2940,7 +2940,7 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11">
       <c r="B13">
         <v>11</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
-    <row r="14" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" ht="28.8">
       <c r="B14">
         <v>12</v>
       </c>
@@ -2994,7 +2994,7 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11">
       <c r="B15">
         <v>13</v>
       </c>
@@ -3021,7 +3021,7 @@
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11">
       <c r="B16">
         <v>14</v>
       </c>
@@ -3048,7 +3048,7 @@
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11">
       <c r="B17">
         <v>15</v>
       </c>
@@ -3075,7 +3075,7 @@
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11">
       <c r="D18" t="str">
         <f>CONCATENATE(Personal!B19, ,Personal!C19,  ,Personal!D19)</f>
         <v/>
@@ -3100,7 +3100,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16.21875" customWidth="1"/>
     <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
@@ -3121,7 +3121,7 @@
     <col min="17" max="17" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="B2" s="18" t="s">
         <v>180</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17">
       <c r="G18" s="4"/>
     </row>
   </sheetData>
@@ -3877,11 +3877,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4:L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
@@ -3901,7 +3901,7 @@
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="B2" s="15" t="s">
         <v>231</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>15</v>
       </c>

</xml_diff>